<commit_message>
Update NULL race as others
</commit_message>
<xml_diff>
--- a/data/CARES_fields_info.xlsx
+++ b/data/CARES_fields_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardow41/Dev/SMU/CARES_Analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F29F4F-E886-034B-B21D-290669090BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2987C3-5298-F24D-91B6-965EF1896268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{36653A06-9A8A-4536-9238-602EC8D8D6A8}"/>
   </bookViews>
@@ -269,9 +269,6 @@
     <t>combined moderate and severity</t>
   </si>
   <si>
-    <t>null as NaN (instead of changing NULL to Others)</t>
-  </si>
-  <si>
     <t>null as class NO</t>
   </si>
   <si>
@@ -300,6 +297,9 @@
   </si>
   <si>
     <t>null as class NO (because RCRI is also not tested)</t>
+  </si>
+  <si>
+    <t>null as "Others" race</t>
   </si>
 </sst>
 </file>
@@ -789,13 +789,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1607,7 +1605,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1618,437 +1616,437 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="D8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D19"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="4" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="3" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="D33" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Data Preparation for ignored columns
</commit_message>
<xml_diff>
--- a/data/CARES_fields_info.xlsx
+++ b/data/CARES_fields_info.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardow41/Dev/SMU/CARES_Analytics/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Singapore Management University\SMU Singapore\Academics\Jul 2024\Applied Healthcare Analytics\CARES_Analytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2987C3-5298-F24D-91B6-965EF1896268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E751F5D9-6356-41F1-BD83-7CFCE9DC6D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{36653A06-9A8A-4536-9238-602EC8D8D6A8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{36653A06-9A8A-4536-9238-602EC8D8D6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="CARES_fields_info" sheetId="1" r:id="rId1"/>
     <sheet name="Data Cleaning V1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Data Cleaning V1'!$A$1:$D$33</definedName>
+  </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
@@ -1171,19 +1174,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A90FDD-0C27-4E69-A357-CEB8A07E1FFB}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="2"/>
+    <col min="7" max="7" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1236,7 +1239,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1258,7 +1261,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1299,7 +1302,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1315,7 +1318,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1326,7 +1329,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1337,7 +1340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1348,7 +1351,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1359,7 +1362,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1392,7 +1395,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1403,7 +1406,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1414,7 +1417,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -1430,7 +1433,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1471,7 +1474,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1485,7 +1488,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -1499,7 +1502,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1524,7 +1527,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1535,7 +1538,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -1546,7 +1549,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -1602,20 +1605,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7631281-6DF6-7543-8F10-730764D6EAD5}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1629,7 +1633,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1641,7 +1645,7 @@
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1653,7 +1657,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1667,7 +1671,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1681,7 +1685,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1695,7 +1699,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1707,7 +1711,7 @@
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1719,7 +1723,7 @@
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1731,7 +1735,7 @@
       </c>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1743,7 +1747,7 @@
       </c>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1755,7 +1759,7 @@
       </c>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1767,7 +1771,7 @@
       </c>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1779,7 +1783,7 @@
       </c>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1791,7 +1795,7 @@
       </c>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1803,7 +1807,7 @@
       </c>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1817,7 +1821,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1829,7 +1833,7 @@
       </c>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1843,7 +1847,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1855,7 +1859,7 @@
       </c>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -1869,7 +1873,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -1883,7 +1887,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1897,7 +1901,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1911,7 +1915,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1925,7 +1929,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -1939,7 +1943,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -1953,7 +1957,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1967,7 +1971,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1981,7 +1985,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -1995,7 +1999,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -2007,7 +2011,7 @@
       </c>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -2021,7 +2025,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -2035,7 +2039,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -2049,13 +2053,20 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D33" xr:uid="{C7631281-6DF6-7543-8F10-730764D6EAD5}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="ignored, not used in paper"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Feature engineering for paper ignored columns
</commit_message>
<xml_diff>
--- a/data/CARES_fields_info.xlsx
+++ b/data/CARES_fields_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Singapore Management University\SMU Singapore\Academics\Jul 2024\Applied Healthcare Analytics\CARES_Analytics\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smu-my.sharepoint.com/personal/danieljames_2023_mitb_smu_edu_sg/Documents/SMU Singapore/Academics/Jul 2024/Applied Healthcare Analytics/CARES_Analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E751F5D9-6356-41F1-BD83-7CFCE9DC6D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{36653A06-9A8A-4536-9238-602EC8D8D6A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{36653A06-9A8A-4536-9238-602EC8D8D6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="CARES_fields_info" sheetId="1" r:id="rId1"/>
@@ -1174,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A90FDD-0C27-4E69-A357-CEB8A07E1FFB}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Additional statistical tests and dropping columns in Data Preparation for ignored columns
</commit_message>
<xml_diff>
--- a/data/CARES_fields_info.xlsx
+++ b/data/CARES_fields_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smu-my.sharepoint.com/personal/danieljames_2023_mitb_smu_edu_sg/Documents/SMU Singapore/Academics/Jul 2024/Applied Healthcare Analytics/CARES_Analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E751F5D9-6356-41F1-BD83-7CFCE9DC6D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{E751F5D9-6356-41F1-BD83-7CFCE9DC6D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC741BBB-B267-460B-90BD-F037938596D5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{36653A06-9A8A-4536-9238-602EC8D8D6A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{36653A06-9A8A-4536-9238-602EC8D8D6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="CARES_fields_info" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="99">
   <si>
     <t>Field Name</t>
   </si>
@@ -281,9 +281,6 @@
     <t>Encoding Actions</t>
   </si>
   <si>
-    <t>ignored, not used in paper</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -303,6 +300,27 @@
   </si>
   <si>
     <t>null as "Others" race</t>
+  </si>
+  <si>
+    <t>dropped, could lead to multicollinearity</t>
+  </si>
+  <si>
+    <t>Categorization: preop-eGFR ≤ 98.688 mL/min/1.73 m2 (0) and preop-eGFR &gt; 98.688 mL/min/1.73 m2 (1)</t>
+  </si>
+  <si>
+    <t>Combined into Perioperativetransfusion</t>
+  </si>
+  <si>
+    <t>Label Encoding</t>
+  </si>
+  <si>
+    <t>Label Encoding: Group all three transfusion columns and name the feature as Perioperativetransfusion (1, 0), presence of a single transfusion using OR operation.</t>
+  </si>
+  <si>
+    <t>dropped, as it is redundant</t>
+  </si>
+  <si>
+    <t>Label Encoding: GA-0, RA-1</t>
   </si>
 </sst>
 </file>
@@ -1174,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A90FDD-0C27-4E69-A357-CEB8A07E1FFB}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1605,11 +1623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7631281-6DF6-7543-8F10-730764D6EAD5}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1633,7 +1650,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1645,7 +1662,7 @@
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1657,7 +1674,7 @@
       </c>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1668,7 +1685,7 @@
         <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1679,13 +1696,13 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1696,7 +1713,7 @@
         <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1707,11 +1724,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7"/>
-    </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1723,7 +1742,7 @@
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1735,7 +1754,7 @@
       </c>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1755,9 +1774,11 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11"/>
+        <v>94</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1767,9 +1788,11 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12"/>
+        <v>94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1779,9 +1802,11 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13"/>
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1791,7 +1816,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D14"/>
     </row>
@@ -1803,11 +1828,13 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15"/>
-    </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1818,7 +1845,7 @@
         <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1829,11 +1856,11 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1844,10 +1871,10 @@
         <v>80</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1859,7 +1886,7 @@
       </c>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -1870,10 +1897,10 @@
         <v>80</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -1884,10 +1911,10 @@
         <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1898,10 +1925,10 @@
         <v>80</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1909,13 +1936,13 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1923,13 +1950,13 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -1940,10 +1967,10 @@
         <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -1954,10 +1981,10 @@
         <v>82</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1968,10 +1995,10 @@
         <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1982,10 +2009,10 @@
         <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -1996,10 +2023,10 @@
         <v>82</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -2011,7 +2038,7 @@
       </c>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -2022,10 +2049,10 @@
         <v>76</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -2036,10 +2063,10 @@
         <v>76</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -2050,7 +2077,7 @@
         <v>80</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -2060,13 +2087,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D33" xr:uid="{C7631281-6DF6-7543-8F10-730764D6EAD5}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="ignored, not used in paper"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D33" xr:uid="{C7631281-6DF6-7543-8F10-730764D6EAD5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed to Data Preparation Notebooks
</commit_message>
<xml_diff>
--- a/data/CARES_fields_info.xlsx
+++ b/data/CARES_fields_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smu-my.sharepoint.com/personal/danieljames_2023_mitb_smu_edu_sg/Documents/SMU Singapore/Academics/Jul 2024/Applied Healthcare Analytics/CARES_Analytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{E751F5D9-6356-41F1-BD83-7CFCE9DC6D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC741BBB-B267-460B-90BD-F037938596D5}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{E751F5D9-6356-41F1-BD83-7CFCE9DC6D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6F7CD37-B3D9-4965-9E75-EB6D1764E68A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{36653A06-9A8A-4536-9238-602EC8D8D6A8}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Data Cleaning V1'!$A$1:$D$33</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1193,7 +1193,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1623,10 +1623,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7631281-6DF6-7543-8F10-730764D6EAD5}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1650,7 +1651,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1662,7 +1663,7 @@
       </c>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1688,7 +1689,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1730,7 +1731,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1742,7 +1743,7 @@
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1754,7 +1755,7 @@
       </c>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1808,7 +1809,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1848,7 +1849,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1928,7 +1929,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -2026,7 +2027,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -2087,7 +2088,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D33" xr:uid="{C7631281-6DF6-7543-8F10-730764D6EAD5}"/>
+  <autoFilter ref="A1:D33" xr:uid="{C7631281-6DF6-7543-8F10-730764D6EAD5}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="binary, label encoding"/>
+        <filter val="binary, true false to 1 0"/>
+        <filter val="label encoding"/>
+        <filter val="Label Encoding: GA-0, RA-1"/>
+        <filter val="Label Encoding: Group all three transfusion columns and name the feature as Perioperativetransfusion (1, 0), presence of a single transfusion using OR operation."/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>